<commit_message>
fixes import of spanish Start backtrace template
solution: look for a different header, template change

ticket: #455
</commit_message>
<xml_diff>
--- a/de.bund.bfr.knime.openkrise.db/src/de/bund/bfr/knime/openkrise/db/imports/custom/bfrnewformat/FCL_Backtrace_Prod_tob_es.xlsx
+++ b/de.bund.bfr.knime.openkrise.db/src/de/bund/bfr/knime/openkrise/db/imports/custom/bfrnewformat/FCL_Backtrace_Prod_tob_es.xlsx
@@ -102,9 +102,6 @@
     <t>Año</t>
   </si>
   <si>
-    <t>Fecha de recepción</t>
-  </si>
-  <si>
     <t>Por favor, reescriba el lote de la mercancía saliente o la linea que lo identifica en el cuadro inferior tantas veces como sea necesario para obtener todos los ingredientes que la forman.</t>
   </si>
   <si>
@@ -118,6 +115,9 @@
   </si>
   <si>
     <t>En la columna A introduzca a partir de la línea 18 el número de linea de la mercancía de salida a la que esta asociado el ingrediente o su número de lote y rellene los campos desde la columna B en adelante con la información del ingrediente.</t>
+  </si>
+  <si>
+    <t>Fecha de recepción de producto</t>
   </si>
 </sst>
 </file>
@@ -1414,33 +1414,66 @@
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="38" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="38" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="38" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="38" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="38" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="39" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="39" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="39" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="38" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="38" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="38" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="31" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="31" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="31" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="1" fontId="10" fillId="3" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="10" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="30" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="30" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="30" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="10" fillId="30" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="10" fillId="30" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="30" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="12" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1453,32 +1486,16 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="3" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="30" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="30" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="2" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="37" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="37" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="37" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1493,18 +1510,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="37" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="37" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="37" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="49" fontId="36" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1518,6 +1523,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="6" fillId="30" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1532,56 +1540,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="38" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="38" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="38" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="38" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="38" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="39" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="39" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="39" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="38" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="38" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="38" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="31" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="31" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="31" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
+    <xf numFmtId="49" fontId="6" fillId="30" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="30" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="2" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="30" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="30" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="30" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="30" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="30" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="30" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="3" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="114">
@@ -2008,45 +2008,45 @@
   <dimension ref="A1:S41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="C1" sqref="C1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="12.75" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.265625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="25.86328125" style="2" customWidth="1"/>
-    <col min="3" max="4" width="12.3984375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" style="2" customWidth="1"/>
+    <col min="3" max="4" width="12.42578125" style="2" customWidth="1"/>
     <col min="5" max="5" width="12" style="2" customWidth="1"/>
-    <col min="6" max="6" width="4.3984375" style="43" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.73046875" style="43" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.265625" style="43" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.1328125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="21.86328125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="32.73046875" style="2" customWidth="1"/>
-    <col min="12" max="12" width="10.1328125" style="2" customWidth="1"/>
-    <col min="13" max="13" width="11.86328125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="19.265625" style="2" customWidth="1"/>
-    <col min="15" max="19" width="11.3984375" style="1"/>
-    <col min="20" max="16384" width="11.3984375" style="2"/>
+    <col min="6" max="6" width="4.42578125" style="43" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" style="43" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.28515625" style="43" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="21.85546875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="32.7109375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="11.85546875" style="2" customWidth="1"/>
+    <col min="14" max="14" width="19.28515625" style="2" customWidth="1"/>
+    <col min="15" max="19" width="11.42578125" style="1"/>
+    <col min="20" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="11" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="85"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
-      <c r="I1" s="86"/>
-      <c r="J1" s="87"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="52"/>
       <c r="K1" s="8"/>
-      <c r="L1" s="88"/>
-      <c r="M1" s="89"/>
-      <c r="N1" s="90"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="55"/>
       <c r="O1" s="9"/>
       <c r="P1" s="10"/>
       <c r="Q1" s="10"/>
@@ -2054,123 +2054,123 @@
       <c r="S1" s="10"/>
     </row>
     <row r="2" spans="1:19" s="14" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="91" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="92"/>
-      <c r="J2" s="92"/>
-      <c r="K2" s="92"/>
-      <c r="L2" s="92"/>
-      <c r="M2" s="92"/>
-      <c r="N2" s="93"/>
+      <c r="A2" s="56" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="58"/>
       <c r="O2" s="12"/>
       <c r="P2" s="13"/>
       <c r="Q2" s="13"/>
       <c r="R2" s="13"/>
       <c r="S2" s="13"/>
     </row>
-    <row r="3" spans="1:19" s="16" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="54" t="s">
+    <row r="3" spans="1:19" s="16" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="62" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="55"/>
-      <c r="L3" s="55"/>
-      <c r="M3" s="56"/>
-      <c r="N3" s="57"/>
+      <c r="B3" s="63"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="63"/>
+      <c r="L3" s="63"/>
+      <c r="M3" s="64"/>
+      <c r="N3" s="65"/>
       <c r="O3" s="15"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
     </row>
-    <row r="4" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="47" t="s">
+      <c r="B4" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47" t="s">
+      <c r="C4" s="76"/>
+      <c r="D4" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="47"/>
-      <c r="F4" s="58" t="s">
+      <c r="E4" s="76"/>
+      <c r="F4" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="58"/>
-      <c r="H4" s="58"/>
-      <c r="I4" s="58"/>
-      <c r="J4" s="77" t="s">
+      <c r="G4" s="59"/>
+      <c r="H4" s="59"/>
+      <c r="I4" s="59"/>
+      <c r="J4" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="K4" s="78"/>
-      <c r="L4" s="78"/>
-      <c r="M4" s="79"/>
+      <c r="K4" s="79"/>
+      <c r="L4" s="79"/>
+      <c r="M4" s="80"/>
       <c r="N4" s="72" t="s">
         <v>21</v>
       </c>
       <c r="O4" s="15"/>
     </row>
-    <row r="5" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="74"/>
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="47" t="s">
+      <c r="C5" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="47" t="s">
+      <c r="D5" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="47" t="s">
+      <c r="E5" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="58" t="s">
+      <c r="F5" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="58"/>
-      <c r="H5" s="58"/>
-      <c r="I5" s="47" t="s">
+      <c r="G5" s="59"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="J5" s="65" t="s">
+      <c r="J5" s="86" t="s">
         <v>5</v>
       </c>
-      <c r="K5" s="65" t="s">
+      <c r="K5" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="L5" s="65" t="s">
+      <c r="L5" s="86" t="s">
         <v>15</v>
       </c>
-      <c r="M5" s="63" t="s">
+      <c r="M5" s="84" t="s">
         <v>14</v>
       </c>
       <c r="N5" s="72"/>
       <c r="O5" s="15"/>
     </row>
-    <row r="6" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="75"/>
-      <c r="B6" s="47"/>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
+      <c r="B6" s="76"/>
+      <c r="C6" s="76"/>
+      <c r="D6" s="76"/>
+      <c r="E6" s="76"/>
       <c r="F6" s="6" t="s">
         <v>10</v>
       </c>
@@ -2180,11 +2180,11 @@
       <c r="H6" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="I6" s="47"/>
-      <c r="J6" s="65"/>
-      <c r="K6" s="65"/>
-      <c r="L6" s="65"/>
-      <c r="M6" s="64"/>
+      <c r="I6" s="76"/>
+      <c r="J6" s="86"/>
+      <c r="K6" s="86"/>
+      <c r="L6" s="86"/>
+      <c r="M6" s="85"/>
       <c r="N6" s="72"/>
       <c r="O6" s="15"/>
     </row>
@@ -2212,157 +2212,157 @@
       <c r="S7" s="1"/>
     </row>
     <row r="8" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="69" t="s">
+      <c r="A8" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="70"/>
-      <c r="C8" s="70"/>
-      <c r="D8" s="70"/>
-      <c r="E8" s="70"/>
-      <c r="F8" s="70"/>
-      <c r="G8" s="70"/>
-      <c r="H8" s="70"/>
-      <c r="I8" s="70"/>
-      <c r="J8" s="70"/>
-      <c r="K8" s="70"/>
-      <c r="L8" s="70"/>
-      <c r="M8" s="70"/>
-      <c r="N8" s="71"/>
-    </row>
-    <row r="9" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="66" t="s">
+      <c r="B8" s="67"/>
+      <c r="C8" s="67"/>
+      <c r="D8" s="67"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="67"/>
+      <c r="H8" s="67"/>
+      <c r="I8" s="67"/>
+      <c r="J8" s="67"/>
+      <c r="K8" s="67"/>
+      <c r="L8" s="67"/>
+      <c r="M8" s="67"/>
+      <c r="N8" s="68"/>
+    </row>
+    <row r="9" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="69" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="70"/>
+      <c r="C9" s="70"/>
+      <c r="D9" s="70"/>
+      <c r="E9" s="70"/>
+      <c r="F9" s="70"/>
+      <c r="G9" s="70"/>
+      <c r="H9" s="70"/>
+      <c r="I9" s="70"/>
+      <c r="J9" s="70"/>
+      <c r="K9" s="70"/>
+      <c r="L9" s="70"/>
+      <c r="M9" s="70"/>
+      <c r="N9" s="71"/>
+    </row>
+    <row r="10" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="69" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="70"/>
+      <c r="C10" s="70"/>
+      <c r="D10" s="70"/>
+      <c r="E10" s="70"/>
+      <c r="F10" s="70"/>
+      <c r="G10" s="70"/>
+      <c r="H10" s="70"/>
+      <c r="I10" s="70"/>
+      <c r="J10" s="70"/>
+      <c r="K10" s="70"/>
+      <c r="L10" s="70"/>
+      <c r="M10" s="70"/>
+      <c r="N10" s="71"/>
+    </row>
+    <row r="11" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="69" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="70"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="70"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="70"/>
+      <c r="H11" s="70"/>
+      <c r="I11" s="70"/>
+      <c r="J11" s="70"/>
+      <c r="K11" s="70"/>
+      <c r="L11" s="70"/>
+      <c r="M11" s="70"/>
+      <c r="N11" s="71"/>
+    </row>
+    <row r="12" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="69" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="70"/>
+      <c r="C12" s="70"/>
+      <c r="D12" s="70"/>
+      <c r="E12" s="70"/>
+      <c r="F12" s="70"/>
+      <c r="G12" s="70"/>
+      <c r="H12" s="70"/>
+      <c r="I12" s="70"/>
+      <c r="J12" s="70"/>
+      <c r="K12" s="70"/>
+      <c r="L12" s="70"/>
+      <c r="M12" s="70"/>
+      <c r="N12" s="71"/>
+    </row>
+    <row r="13" spans="1:19" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="67"/>
-      <c r="C9" s="67"/>
-      <c r="D9" s="67"/>
-      <c r="E9" s="67"/>
-      <c r="F9" s="67"/>
-      <c r="G9" s="67"/>
-      <c r="H9" s="67"/>
-      <c r="I9" s="67"/>
-      <c r="J9" s="67"/>
-      <c r="K9" s="67"/>
-      <c r="L9" s="67"/>
-      <c r="M9" s="67"/>
-      <c r="N9" s="68"/>
-    </row>
-    <row r="10" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="66" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="67"/>
-      <c r="C10" s="67"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="67"/>
-      <c r="F10" s="67"/>
-      <c r="G10" s="67"/>
-      <c r="H10" s="67"/>
-      <c r="I10" s="67"/>
-      <c r="J10" s="67"/>
-      <c r="K10" s="67"/>
-      <c r="L10" s="67"/>
-      <c r="M10" s="67"/>
-      <c r="N10" s="68"/>
-    </row>
-    <row r="11" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="66" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="67"/>
-      <c r="C11" s="67"/>
-      <c r="D11" s="67"/>
-      <c r="E11" s="67"/>
-      <c r="F11" s="67"/>
-      <c r="G11" s="67"/>
-      <c r="H11" s="67"/>
-      <c r="I11" s="67"/>
-      <c r="J11" s="67"/>
-      <c r="K11" s="67"/>
-      <c r="L11" s="67"/>
-      <c r="M11" s="67"/>
-      <c r="N11" s="68"/>
-    </row>
-    <row r="12" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="66" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="67"/>
-      <c r="C12" s="67"/>
-      <c r="D12" s="67"/>
-      <c r="E12" s="67"/>
-      <c r="F12" s="67"/>
-      <c r="G12" s="67"/>
-      <c r="H12" s="67"/>
-      <c r="I12" s="67"/>
-      <c r="J12" s="67"/>
-      <c r="K12" s="67"/>
-      <c r="L12" s="67"/>
-      <c r="M12" s="67"/>
-      <c r="N12" s="68"/>
-    </row>
-    <row r="13" spans="1:19" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A13" s="66" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="67"/>
-      <c r="C13" s="67"/>
-      <c r="D13" s="67"/>
-      <c r="E13" s="67"/>
-      <c r="F13" s="67"/>
-      <c r="G13" s="67"/>
-      <c r="H13" s="67"/>
-      <c r="I13" s="67"/>
-      <c r="J13" s="67"/>
-      <c r="K13" s="67"/>
-      <c r="L13" s="67"/>
-      <c r="M13" s="67"/>
-      <c r="N13" s="68"/>
-    </row>
-    <row r="14" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="54" t="s">
+      <c r="B13" s="70"/>
+      <c r="C13" s="70"/>
+      <c r="D13" s="70"/>
+      <c r="E13" s="70"/>
+      <c r="F13" s="70"/>
+      <c r="G13" s="70"/>
+      <c r="H13" s="70"/>
+      <c r="I13" s="70"/>
+      <c r="J13" s="70"/>
+      <c r="K13" s="70"/>
+      <c r="L13" s="70"/>
+      <c r="M13" s="70"/>
+      <c r="N13" s="71"/>
+    </row>
+    <row r="14" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="55"/>
-      <c r="C14" s="55"/>
-      <c r="D14" s="55"/>
-      <c r="E14" s="55"/>
-      <c r="F14" s="55"/>
-      <c r="G14" s="55"/>
-      <c r="H14" s="55"/>
-      <c r="I14" s="55"/>
-      <c r="J14" s="55"/>
-      <c r="K14" s="55"/>
-      <c r="L14" s="55"/>
-      <c r="M14" s="56"/>
-      <c r="N14" s="57"/>
+      <c r="B14" s="63"/>
+      <c r="C14" s="63"/>
+      <c r="D14" s="63"/>
+      <c r="E14" s="63"/>
+      <c r="F14" s="63"/>
+      <c r="G14" s="63"/>
+      <c r="H14" s="63"/>
+      <c r="I14" s="63"/>
+      <c r="J14" s="63"/>
+      <c r="K14" s="63"/>
+      <c r="L14" s="63"/>
+      <c r="M14" s="64"/>
+      <c r="N14" s="65"/>
       <c r="O14" s="15"/>
       <c r="P14" s="44"/>
     </row>
-    <row r="15" spans="1:19" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:19" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="59" t="s">
+      <c r="B15" s="93" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="59"/>
-      <c r="D15" s="76" t="s">
+      <c r="C15" s="93"/>
+      <c r="D15" s="77" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="76"/>
-      <c r="F15" s="53" t="s">
+      <c r="E15" s="77"/>
+      <c r="F15" s="92" t="s">
         <v>8</v>
       </c>
-      <c r="G15" s="53"/>
-      <c r="H15" s="53"/>
-      <c r="I15" s="53"/>
-      <c r="J15" s="60" t="s">
+      <c r="G15" s="92"/>
+      <c r="H15" s="92"/>
+      <c r="I15" s="92"/>
+      <c r="J15" s="81" t="s">
         <v>25</v>
       </c>
-      <c r="K15" s="61"/>
-      <c r="L15" s="61"/>
-      <c r="M15" s="62"/>
+      <c r="K15" s="82"/>
+      <c r="L15" s="82"/>
+      <c r="M15" s="83"/>
       <c r="N15" s="72" t="s">
         <v>21</v>
       </c>
@@ -2372,38 +2372,38 @@
       <c r="R15" s="4"/>
       <c r="S15" s="4"/>
     </row>
-    <row r="16" spans="1:19" s="5" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:19" s="5" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="74"/>
-      <c r="B16" s="45" t="s">
+      <c r="B16" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="45" t="s">
+      <c r="C16" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="D16" s="45" t="s">
+      <c r="D16" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="45" t="s">
+      <c r="E16" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="F16" s="48" t="s">
-        <v>27</v>
-      </c>
-      <c r="G16" s="49"/>
-      <c r="H16" s="50"/>
-      <c r="I16" s="51" t="s">
+      <c r="F16" s="87" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" s="88"/>
+      <c r="H16" s="89"/>
+      <c r="I16" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="J16" s="45" t="s">
+      <c r="J16" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="K16" s="45" t="s">
+      <c r="K16" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="L16" s="45" t="s">
+      <c r="L16" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="M16" s="45" t="s">
+      <c r="M16" s="60" t="s">
         <v>14</v>
       </c>
       <c r="N16" s="72"/>
@@ -2413,12 +2413,12 @@
       <c r="R16" s="4"/>
       <c r="S16" s="4"/>
     </row>
-    <row r="17" spans="1:19" s="5" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:19" s="5" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="75"/>
-      <c r="B17" s="46"/>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
+      <c r="B17" s="61"/>
+      <c r="C17" s="61"/>
+      <c r="D17" s="61"/>
+      <c r="E17" s="61"/>
       <c r="F17" s="7" t="s">
         <v>10</v>
       </c>
@@ -2428,11 +2428,11 @@
       <c r="H17" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="I17" s="52"/>
-      <c r="J17" s="46"/>
-      <c r="K17" s="46"/>
-      <c r="L17" s="46"/>
-      <c r="M17" s="46"/>
+      <c r="I17" s="91"/>
+      <c r="J17" s="61"/>
+      <c r="K17" s="61"/>
+      <c r="L17" s="61"/>
+      <c r="M17" s="61"/>
       <c r="N17" s="72"/>
       <c r="O17" s="3"/>
       <c r="P17" s="4"/>
@@ -2831,7 +2831,7 @@
       <c r="N40" s="36"/>
       <c r="O40" s="15"/>
     </row>
-    <row r="41" spans="1:15" ht="13.15" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="38"/>
       <c r="B41" s="39"/>
       <c r="C41" s="39"/>
@@ -2850,11 +2850,30 @@
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="L1:N1"/>
-    <mergeCell ref="A2:N2"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="L16:L17"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="A14:N14"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="J15:M15"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="A12:N12"/>
+    <mergeCell ref="A13:N13"/>
+    <mergeCell ref="I5:I6"/>
     <mergeCell ref="F4:I4"/>
     <mergeCell ref="M16:M17"/>
     <mergeCell ref="A3:N3"/>
@@ -2871,30 +2890,11 @@
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="J4:M4"/>
-    <mergeCell ref="J15:M15"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="A12:N12"/>
-    <mergeCell ref="A13:N13"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="K16:K17"/>
-    <mergeCell ref="L16:L17"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="A14:N14"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="A2:N2"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F7 F14 F3 F18:F1048576">

</xml_diff>